<commit_message>
this is my new commit
</commit_message>
<xml_diff>
--- a/src/test/java/Testdata/Exceldata.xlsx
+++ b/src/test/java/Testdata/Exceldata.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14160" windowHeight="3060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -24,9 +25,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>mahesh23456</t>
-  </si>
-  <si>
     <t>India@123</t>
   </si>
   <si>
@@ -37,6 +35,12 @@
   </si>
   <si>
     <t>mohan@456</t>
+  </si>
+  <si>
+    <t>naveen2747</t>
+  </si>
+  <si>
+    <t>Tester@2747</t>
   </si>
 </sst>
 </file>
@@ -417,7 +421,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,26 +440,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>